<commit_message>
Modèle univrié sans IC
</commit_message>
<xml_diff>
--- a/Results.xlsx
+++ b/Results.xlsx
@@ -4136,7 +4136,7 @@
     <t>0.133</t>
   </si>
   <si>
-    <t>0.951‡</t>
+    <t>0.935‡</t>
   </si>
   <si>
     <t>0.885</t>
@@ -4175,28 +4175,28 @@
     <t>0.8</t>
   </si>
   <si>
-    <t>0.347‡</t>
+    <t>0.362‡</t>
   </si>
   <si>
     <t>5e-04‡</t>
   </si>
   <si>
-    <t>0.032‡</t>
+    <t>0.03‡</t>
   </si>
   <si>
     <t>0.00109</t>
   </si>
   <si>
-    <t>0.844‡</t>
-  </si>
-  <si>
-    <t>0.002‡</t>
+    <t>0.841‡</t>
+  </si>
+  <si>
+    <t>0.0015‡</t>
   </si>
   <si>
     <t>0.0412</t>
   </si>
   <si>
-    <t>0.91‡</t>
+    <t>0.916‡</t>
   </si>
   <si>
     <t>2.9e-59</t>
@@ -4208,19 +4208,19 @@
     <t>1.46e-05</t>
   </si>
   <si>
-    <t>0.0285‡</t>
+    <t>0.034‡</t>
   </si>
   <si>
     <t>0.285</t>
   </si>
   <si>
-    <t>0.71‡</t>
+    <t>0.714‡</t>
   </si>
   <si>
     <t>0.19</t>
   </si>
   <si>
-    <t>0.0495‡</t>
+    <t>0.045‡</t>
   </si>
   <si>
     <t>1.05e-06</t>
@@ -4292,7 +4292,7 @@
     <t>0.0885</t>
   </si>
   <si>
-    <t>0.357‡</t>
+    <t>0.367‡</t>
   </si>
   <si>
     <t>6.56e-07</t>
@@ -4337,7 +4337,7 @@
     <t>0.322</t>
   </si>
   <si>
-    <t>0.649‡</t>
+    <t>0.653‡</t>
   </si>
   <si>
     <t>0.0718</t>
@@ -4367,7 +4367,7 @@
     <t>0.648</t>
   </si>
   <si>
-    <t>0.386‡</t>
+    <t>0.388‡</t>
   </si>
   <si>
     <t>0.653</t>
@@ -4376,13 +4376,16 @@
     <t>0.734</t>
   </si>
   <si>
-    <t>0.473‡</t>
-  </si>
-  <si>
-    <t>0.0015‡</t>
-  </si>
-  <si>
-    <t>0.615‡</t>
+    <t>0.491‡</t>
+  </si>
+  <si>
+    <t>0.001‡</t>
+  </si>
+  <si>
+    <t>0.0025‡</t>
+  </si>
+  <si>
+    <t>0.571‡</t>
   </si>
   <si>
     <t>0.726</t>
@@ -4412,7 +4415,7 @@
     <t>0.0462</t>
   </si>
   <si>
-    <t>0.403‡</t>
+    <t>0.395‡</t>
   </si>
   <si>
     <t>0.104</t>
@@ -4424,10 +4427,10 @@
     <t>0.000453</t>
   </si>
   <si>
-    <t>0.0125‡</t>
-  </si>
-  <si>
-    <t>0.004‡</t>
+    <t>0.0145‡</t>
+  </si>
+  <si>
+    <t>0.0045‡</t>
   </si>
   <si>
     <t>0.33</t>
@@ -4439,16 +4442,13 @@
     <t>0.182</t>
   </si>
   <si>
-    <t>0.001‡</t>
-  </si>
-  <si>
     <t>0.00629</t>
   </si>
   <si>
     <t>0.421</t>
   </si>
   <si>
-    <t>0.74‡</t>
+    <t>0.744‡</t>
   </si>
   <si>
     <t>0.00408</t>
@@ -4457,7 +4457,7 @@
     <t>0.00646</t>
   </si>
   <si>
-    <t>0.323‡</t>
+    <t>0.337‡</t>
   </si>
   <si>
     <t>4.08e-19</t>
@@ -11694,7 +11694,7 @@
         <v>554</v>
       </c>
       <c r="D509" t="s">
-        <v>1392</v>
+        <v>1456</v>
       </c>
     </row>
     <row r="510">
@@ -11778,7 +11778,7 @@
         <v>554</v>
       </c>
       <c r="D515" t="s">
-        <v>1456</v>
+        <v>1457</v>
       </c>
     </row>
     <row r="516">
@@ -12170,7 +12170,7 @@
         <v>1262</v>
       </c>
       <c r="D543" t="s">
-        <v>1457</v>
+        <v>1458</v>
       </c>
     </row>
     <row r="544">
@@ -12212,7 +12212,7 @@
         <v>1263</v>
       </c>
       <c r="D546" t="s">
-        <v>1458</v>
+        <v>1459</v>
       </c>
     </row>
     <row r="547">
@@ -12254,7 +12254,7 @@
         <v>554</v>
       </c>
       <c r="D549" t="s">
-        <v>1459</v>
+        <v>1460</v>
       </c>
     </row>
     <row r="550">
@@ -12338,7 +12338,7 @@
         <v>1269</v>
       </c>
       <c r="D555" t="s">
-        <v>1460</v>
+        <v>1461</v>
       </c>
     </row>
     <row r="556">
@@ -12352,7 +12352,7 @@
         <v>1270</v>
       </c>
       <c r="D556" t="s">
-        <v>1461</v>
+        <v>1462</v>
       </c>
     </row>
     <row r="557">
@@ -12366,7 +12366,7 @@
         <v>1271</v>
       </c>
       <c r="D557" t="s">
-        <v>1462</v>
+        <v>1463</v>
       </c>
     </row>
     <row r="558">
@@ -12380,7 +12380,7 @@
         <v>1272</v>
       </c>
       <c r="D558" t="s">
-        <v>1463</v>
+        <v>1464</v>
       </c>
     </row>
     <row r="559">
@@ -12408,7 +12408,7 @@
         <v>554</v>
       </c>
       <c r="D560" t="s">
-        <v>1464</v>
+        <v>1465</v>
       </c>
     </row>
     <row r="561">
@@ -12464,7 +12464,7 @@
         <v>554</v>
       </c>
       <c r="D564" t="s">
-        <v>1465</v>
+        <v>1466</v>
       </c>
     </row>
     <row r="565">
@@ -12520,7 +12520,7 @@
         <v>554</v>
       </c>
       <c r="D568" t="s">
-        <v>1466</v>
+        <v>1467</v>
       </c>
     </row>
     <row r="569">
@@ -12576,7 +12576,7 @@
         <v>554</v>
       </c>
       <c r="D572" t="s">
-        <v>1467</v>
+        <v>1468</v>
       </c>
     </row>
     <row r="573">
@@ -12632,7 +12632,7 @@
         <v>554</v>
       </c>
       <c r="D576" t="s">
-        <v>1468</v>
+        <v>1469</v>
       </c>
     </row>
     <row r="577">
@@ -12688,7 +12688,7 @@
         <v>554</v>
       </c>
       <c r="D580" t="s">
-        <v>1469</v>
+        <v>1470</v>
       </c>
     </row>
     <row r="581">
@@ -12744,7 +12744,7 @@
         <v>554</v>
       </c>
       <c r="D584" t="s">
-        <v>1470</v>
+        <v>1471</v>
       </c>
     </row>
     <row r="585">
@@ -12800,7 +12800,7 @@
         <v>554</v>
       </c>
       <c r="D588" t="s">
-        <v>1471</v>
+        <v>1472</v>
       </c>
     </row>
     <row r="589">
@@ -12856,7 +12856,7 @@
         <v>554</v>
       </c>
       <c r="D592" t="s">
-        <v>1472</v>
+        <v>1473</v>
       </c>
     </row>
     <row r="593">
@@ -12912,7 +12912,7 @@
         <v>554</v>
       </c>
       <c r="D596" t="s">
-        <v>1473</v>
+        <v>1474</v>
       </c>
     </row>
     <row r="597">
@@ -12968,7 +12968,7 @@
         <v>554</v>
       </c>
       <c r="D600" t="s">
-        <v>1474</v>
+        <v>1475</v>
       </c>
     </row>
     <row r="601">
@@ -13024,7 +13024,7 @@
         <v>554</v>
       </c>
       <c r="D604" t="s">
-        <v>1475</v>
+        <v>1388</v>
       </c>
     </row>
     <row r="605">

</xml_diff>

<commit_message>
V1.10 fonctionnelle Utilisation de logistf
</commit_message>
<xml_diff>
--- a/Results.xlsx
+++ b/Results.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2836" uniqueCount="1503">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2836" uniqueCount="1502">
   <si>
     <t>characteristics</t>
   </si>
@@ -4136,7 +4136,7 @@
     <t>0.133</t>
   </si>
   <si>
-    <t>0.947‡</t>
+    <t>0.95‡</t>
   </si>
   <si>
     <t>0.885</t>
@@ -4175,246 +4175,246 @@
     <t>0.8</t>
   </si>
   <si>
-    <t>0.352‡</t>
+    <t>0.361‡</t>
   </si>
   <si>
     <t>5e-04‡</t>
   </si>
   <si>
-    <t>0.0275‡</t>
+    <t>0.0265‡</t>
   </si>
   <si>
     <t>0.00109</t>
   </si>
   <si>
-    <t>0.849‡</t>
+    <t>0.847‡</t>
+  </si>
+  <si>
+    <t>0.0412</t>
+  </si>
+  <si>
+    <t>0.001‡</t>
+  </si>
+  <si>
+    <t>0.899‡</t>
+  </si>
+  <si>
+    <t>2.9e-59</t>
+  </si>
+  <si>
+    <t>2.5e-88</t>
+  </si>
+  <si>
+    <t>1.46e-05</t>
+  </si>
+  <si>
+    <t>0.025‡</t>
+  </si>
+  <si>
+    <t>0.285</t>
+  </si>
+  <si>
+    <t>0.737‡</t>
+  </si>
+  <si>
+    <t>0.19</t>
+  </si>
+  <si>
+    <t>0.047‡</t>
+  </si>
+  <si>
+    <t>1.05e-06</t>
+  </si>
+  <si>
+    <t>0.0406</t>
+  </si>
+  <si>
+    <t>6.79e-05</t>
+  </si>
+  <si>
+    <t>8.58e-07</t>
+  </si>
+  <si>
+    <t>0.0489</t>
+  </si>
+  <si>
+    <t>0.632</t>
+  </si>
+  <si>
+    <t>0.0225</t>
+  </si>
+  <si>
+    <t>0.101</t>
+  </si>
+  <si>
+    <t>7.71e-16</t>
+  </si>
+  <si>
+    <t>0.644</t>
+  </si>
+  <si>
+    <t>1.43e-14</t>
+  </si>
+  <si>
+    <t>5.63e-13</t>
+  </si>
+  <si>
+    <t>0.955</t>
+  </si>
+  <si>
+    <t>2.14e-13</t>
+  </si>
+  <si>
+    <t>0.0565</t>
+  </si>
+  <si>
+    <t>0.00294</t>
+  </si>
+  <si>
+    <t>0.087</t>
+  </si>
+  <si>
+    <t>0.311</t>
+  </si>
+  <si>
+    <t>0.0257</t>
+  </si>
+  <si>
+    <t>0.055</t>
+  </si>
+  <si>
+    <t>0.0707</t>
+  </si>
+  <si>
+    <t>1.81e-06</t>
+  </si>
+  <si>
+    <t>0.0885</t>
+  </si>
+  <si>
+    <t>0.332‡</t>
+  </si>
+  <si>
+    <t>6.56e-07</t>
+  </si>
+  <si>
+    <t>0.0377</t>
+  </si>
+  <si>
+    <t>0.0758</t>
+  </si>
+  <si>
+    <t>4.16e-12</t>
+  </si>
+  <si>
+    <t>0.00935</t>
+  </si>
+  <si>
+    <t>0.206</t>
+  </si>
+  <si>
+    <t>0.799</t>
+  </si>
+  <si>
+    <t>0.532</t>
+  </si>
+  <si>
+    <t>0.949</t>
+  </si>
+  <si>
+    <t>0.37</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>0.997</t>
+  </si>
+  <si>
+    <t>0.807</t>
+  </si>
+  <si>
+    <t>0.322</t>
+  </si>
+  <si>
+    <t>0.623‡</t>
+  </si>
+  <si>
+    <t>0.0718</t>
+  </si>
+  <si>
+    <t>0.125</t>
+  </si>
+  <si>
+    <t>0.975</t>
+  </si>
+  <si>
+    <t>0.711‡</t>
+  </si>
+  <si>
+    <t>0.381‡</t>
+  </si>
+  <si>
+    <t>0.517‡</t>
+  </si>
+  <si>
+    <t>0.131‡</t>
+  </si>
+  <si>
+    <t>0.0335‡</t>
+  </si>
+  <si>
+    <t>0.648</t>
+  </si>
+  <si>
+    <t>0.398‡</t>
+  </si>
+  <si>
+    <t>0.653</t>
+  </si>
+  <si>
+    <t>0.734</t>
+  </si>
+  <si>
+    <t>0.468‡</t>
   </si>
   <si>
     <t>0.002‡</t>
   </si>
   <si>
-    <t>0.0412</t>
-  </si>
-  <si>
-    <t>0.92‡</t>
-  </si>
-  <si>
-    <t>2.9e-59</t>
-  </si>
-  <si>
-    <t>2.5e-88</t>
-  </si>
-  <si>
-    <t>1.46e-05</t>
-  </si>
-  <si>
-    <t>0.03‡</t>
-  </si>
-  <si>
-    <t>0.285</t>
-  </si>
-  <si>
-    <t>0.73‡</t>
-  </si>
-  <si>
-    <t>0.19</t>
-  </si>
-  <si>
-    <t>0.0515‡</t>
-  </si>
-  <si>
-    <t>1.05e-06</t>
-  </si>
-  <si>
-    <t>0.0406</t>
-  </si>
-  <si>
-    <t>6.79e-05</t>
-  </si>
-  <si>
-    <t>8.58e-07</t>
-  </si>
-  <si>
-    <t>0.0489</t>
-  </si>
-  <si>
-    <t>0.632</t>
-  </si>
-  <si>
-    <t>0.0225</t>
-  </si>
-  <si>
-    <t>0.101</t>
-  </si>
-  <si>
-    <t>7.71e-16</t>
-  </si>
-  <si>
-    <t>0.644</t>
-  </si>
-  <si>
-    <t>1.43e-14</t>
-  </si>
-  <si>
-    <t>5.63e-13</t>
-  </si>
-  <si>
-    <t>0.955</t>
-  </si>
-  <si>
-    <t>2.14e-13</t>
-  </si>
-  <si>
-    <t>0.0565</t>
-  </si>
-  <si>
-    <t>0.00294</t>
-  </si>
-  <si>
-    <t>0.087</t>
-  </si>
-  <si>
-    <t>0.311</t>
-  </si>
-  <si>
-    <t>0.0257</t>
-  </si>
-  <si>
-    <t>0.055</t>
-  </si>
-  <si>
-    <t>0.0707</t>
-  </si>
-  <si>
-    <t>1.81e-06</t>
-  </si>
-  <si>
-    <t>0.0885</t>
-  </si>
-  <si>
-    <t>0.355‡</t>
-  </si>
-  <si>
-    <t>6.56e-07</t>
-  </si>
-  <si>
-    <t>0.0377</t>
-  </si>
-  <si>
-    <t>0.0758</t>
-  </si>
-  <si>
-    <t>4.16e-12</t>
-  </si>
-  <si>
-    <t>0.00935</t>
-  </si>
-  <si>
-    <t>0.206</t>
-  </si>
-  <si>
-    <t>0.799</t>
-  </si>
-  <si>
-    <t>0.532</t>
-  </si>
-  <si>
-    <t>0.949</t>
-  </si>
-  <si>
-    <t>0.37</t>
-  </si>
-  <si>
-    <t>1</t>
-  </si>
-  <si>
-    <t>0.997</t>
-  </si>
-  <si>
-    <t>0.807</t>
-  </si>
-  <si>
-    <t>0.322</t>
-  </si>
-  <si>
-    <t>0.635‡</t>
-  </si>
-  <si>
-    <t>0.0718</t>
-  </si>
-  <si>
-    <t>0.125</t>
-  </si>
-  <si>
-    <t>0.975</t>
-  </si>
-  <si>
-    <t>0.711‡</t>
-  </si>
-  <si>
-    <t>0.381‡</t>
-  </si>
-  <si>
-    <t>0.517‡</t>
-  </si>
-  <si>
-    <t>0.131‡</t>
-  </si>
-  <si>
-    <t>0.0335‡</t>
-  </si>
-  <si>
-    <t>0.648</t>
+    <t>0.606‡</t>
+  </si>
+  <si>
+    <t>0.726</t>
+  </si>
+  <si>
+    <t>1.94e-78</t>
+  </si>
+  <si>
+    <t>1.2e-22</t>
+  </si>
+  <si>
+    <t>0.00114</t>
+  </si>
+  <si>
+    <t>0.0936</t>
+  </si>
+  <si>
+    <t>0.000733</t>
+  </si>
+  <si>
+    <t>0.524</t>
+  </si>
+  <si>
+    <t>0.033</t>
+  </si>
+  <si>
+    <t>0.0462</t>
   </si>
   <si>
     <t>0.402‡</t>
   </si>
   <si>
-    <t>0.653</t>
-  </si>
-  <si>
-    <t>0.734</t>
-  </si>
-  <si>
-    <t>0.491‡</t>
-  </si>
-  <si>
-    <t>0.0015‡</t>
-  </si>
-  <si>
-    <t>0.589‡</t>
-  </si>
-  <si>
-    <t>0.726</t>
-  </si>
-  <si>
-    <t>1.94e-78</t>
-  </si>
-  <si>
-    <t>1.2e-22</t>
-  </si>
-  <si>
-    <t>0.00114</t>
-  </si>
-  <si>
-    <t>0.0936</t>
-  </si>
-  <si>
-    <t>0.000733</t>
-  </si>
-  <si>
-    <t>0.524</t>
-  </si>
-  <si>
-    <t>0.033</t>
-  </si>
-  <si>
-    <t>0.0462</t>
-  </si>
-  <si>
-    <t>0.413‡</t>
-  </si>
-  <si>
     <t>0.104</t>
   </si>
   <si>
@@ -4424,10 +4424,10 @@
     <t>0.000453</t>
   </si>
   <si>
-    <t>0.0155‡</t>
-  </si>
-  <si>
-    <t>0.003‡</t>
+    <t>0.0085‡</t>
+  </si>
+  <si>
+    <t>0.0025‡</t>
   </si>
   <si>
     <t>0.33</t>
@@ -4439,16 +4439,13 @@
     <t>0.182</t>
   </si>
   <si>
-    <t>0.001‡</t>
-  </si>
-  <si>
     <t>0.00629</t>
   </si>
   <si>
     <t>0.421</t>
   </si>
   <si>
-    <t>0.748‡</t>
+    <t>0.761‡</t>
   </si>
   <si>
     <t>0.00408</t>
@@ -4457,7 +4454,7 @@
     <t>0.00646</t>
   </si>
   <si>
-    <t>0.3‡</t>
+    <t>0.315‡</t>
   </si>
   <si>
     <t>4.08e-19</t>
@@ -7116,7 +7113,7 @@
         <v>554</v>
       </c>
       <c r="D182" t="s">
-        <v>1392</v>
+        <v>1388</v>
       </c>
     </row>
     <row r="183">
@@ -7200,7 +7197,7 @@
         <v>1106</v>
       </c>
       <c r="D188" t="s">
-        <v>1393</v>
+        <v>1392</v>
       </c>
     </row>
     <row r="189">
@@ -7368,7 +7365,7 @@
         <v>554</v>
       </c>
       <c r="D200" t="s">
-        <v>1388</v>
+        <v>1393</v>
       </c>
     </row>
     <row r="201">
@@ -8600,7 +8597,7 @@
         <v>554</v>
       </c>
       <c r="D288" t="s">
-        <v>1388</v>
+        <v>1393</v>
       </c>
     </row>
     <row r="289">
@@ -11694,7 +11691,7 @@
         <v>554</v>
       </c>
       <c r="D509" t="s">
-        <v>1392</v>
+        <v>1393</v>
       </c>
     </row>
     <row r="510">
@@ -13024,7 +13021,7 @@
         <v>554</v>
       </c>
       <c r="D604" t="s">
-        <v>1475</v>
+        <v>1455</v>
       </c>
     </row>
     <row r="605">
@@ -13080,7 +13077,7 @@
         <v>554</v>
       </c>
       <c r="D608" t="s">
-        <v>1476</v>
+        <v>1475</v>
       </c>
     </row>
     <row r="609">
@@ -13136,7 +13133,7 @@
         <v>554</v>
       </c>
       <c r="D612" t="s">
-        <v>1477</v>
+        <v>1476</v>
       </c>
     </row>
     <row r="613">
@@ -13192,7 +13189,7 @@
         <v>554</v>
       </c>
       <c r="D616" t="s">
-        <v>1478</v>
+        <v>1477</v>
       </c>
     </row>
     <row r="617">
@@ -13248,7 +13245,7 @@
         <v>554</v>
       </c>
       <c r="D620" t="s">
-        <v>1479</v>
+        <v>1478</v>
       </c>
     </row>
     <row r="621">
@@ -13304,7 +13301,7 @@
         <v>554</v>
       </c>
       <c r="D624" t="s">
-        <v>1480</v>
+        <v>1479</v>
       </c>
     </row>
     <row r="625">
@@ -13360,7 +13357,7 @@
         <v>554</v>
       </c>
       <c r="D628" t="s">
-        <v>1481</v>
+        <v>1480</v>
       </c>
     </row>
     <row r="629">
@@ -13668,7 +13665,7 @@
         <v>554</v>
       </c>
       <c r="D650" t="s">
-        <v>1482</v>
+        <v>1481</v>
       </c>
     </row>
     <row r="651">
@@ -13738,7 +13735,7 @@
         <v>1330</v>
       </c>
       <c r="D655" t="s">
-        <v>1483</v>
+        <v>1482</v>
       </c>
     </row>
     <row r="656">
@@ -13780,7 +13777,7 @@
         <v>1331</v>
       </c>
       <c r="D658" t="s">
-        <v>1484</v>
+        <v>1483</v>
       </c>
     </row>
     <row r="659">
@@ -13822,7 +13819,7 @@
         <v>1332</v>
       </c>
       <c r="D661" t="s">
-        <v>1485</v>
+        <v>1484</v>
       </c>
     </row>
     <row r="662">
@@ -13864,7 +13861,7 @@
         <v>1333</v>
       </c>
       <c r="D664" t="s">
-        <v>1486</v>
+        <v>1485</v>
       </c>
     </row>
     <row r="665">
@@ -13906,7 +13903,7 @@
         <v>554</v>
       </c>
       <c r="D667" t="s">
-        <v>1487</v>
+        <v>1486</v>
       </c>
     </row>
     <row r="668">
@@ -13990,7 +13987,7 @@
         <v>554</v>
       </c>
       <c r="D673" t="s">
-        <v>1487</v>
+        <v>1486</v>
       </c>
     </row>
     <row r="674">
@@ -14046,7 +14043,7 @@
         <v>554</v>
       </c>
       <c r="D677" t="s">
-        <v>1487</v>
+        <v>1486</v>
       </c>
     </row>
     <row r="678">
@@ -14102,7 +14099,7 @@
         <v>1340</v>
       </c>
       <c r="D681" t="s">
-        <v>1488</v>
+        <v>1487</v>
       </c>
     </row>
     <row r="682">
@@ -14116,7 +14113,7 @@
         <v>1339</v>
       </c>
       <c r="D682" t="s">
-        <v>1487</v>
+        <v>1486</v>
       </c>
     </row>
     <row r="683">
@@ -14130,7 +14127,7 @@
         <v>1340</v>
       </c>
       <c r="D683" t="s">
-        <v>1488</v>
+        <v>1487</v>
       </c>
     </row>
     <row r="684">
@@ -14144,7 +14141,7 @@
         <v>1339</v>
       </c>
       <c r="D684" t="s">
-        <v>1487</v>
+        <v>1486</v>
       </c>
     </row>
     <row r="685">
@@ -14158,7 +14155,7 @@
         <v>554</v>
       </c>
       <c r="D685" t="s">
-        <v>1489</v>
+        <v>1488</v>
       </c>
     </row>
     <row r="686">
@@ -14228,7 +14225,7 @@
         <v>1345</v>
       </c>
       <c r="D690" t="s">
-        <v>1490</v>
+        <v>1489</v>
       </c>
     </row>
     <row r="691">
@@ -14242,7 +14239,7 @@
         <v>1346</v>
       </c>
       <c r="D691" t="s">
-        <v>1491</v>
+        <v>1490</v>
       </c>
     </row>
     <row r="692">
@@ -14256,7 +14253,7 @@
         <v>959</v>
       </c>
       <c r="D692" t="s">
-        <v>1488</v>
+        <v>1487</v>
       </c>
     </row>
     <row r="693">
@@ -14270,7 +14267,7 @@
         <v>1347</v>
       </c>
       <c r="D693" t="s">
-        <v>1492</v>
+        <v>1491</v>
       </c>
     </row>
     <row r="694">
@@ -14284,7 +14281,7 @@
         <v>1348</v>
       </c>
       <c r="D694" t="s">
-        <v>1493</v>
+        <v>1492</v>
       </c>
     </row>
     <row r="695">
@@ -14298,7 +14295,7 @@
         <v>959</v>
       </c>
       <c r="D695" t="s">
-        <v>1488</v>
+        <v>1487</v>
       </c>
     </row>
     <row r="696">
@@ -14312,7 +14309,7 @@
         <v>1349</v>
       </c>
       <c r="D696" t="s">
-        <v>1494</v>
+        <v>1493</v>
       </c>
     </row>
     <row r="697">
@@ -14326,7 +14323,7 @@
         <v>1350</v>
       </c>
       <c r="D697" t="s">
-        <v>1495</v>
+        <v>1494</v>
       </c>
     </row>
     <row r="698">
@@ -14340,7 +14337,7 @@
         <v>959</v>
       </c>
       <c r="D698" t="s">
-        <v>1488</v>
+        <v>1487</v>
       </c>
     </row>
     <row r="699">
@@ -14354,7 +14351,7 @@
         <v>1351</v>
       </c>
       <c r="D699" t="s">
-        <v>1496</v>
+        <v>1495</v>
       </c>
     </row>
     <row r="700">
@@ -14368,7 +14365,7 @@
         <v>959</v>
       </c>
       <c r="D700" t="s">
-        <v>1488</v>
+        <v>1487</v>
       </c>
     </row>
     <row r="701">
@@ -14382,7 +14379,7 @@
         <v>1352</v>
       </c>
       <c r="D701" t="s">
-        <v>1497</v>
+        <v>1496</v>
       </c>
     </row>
     <row r="702">
@@ -14396,7 +14393,7 @@
         <v>959</v>
       </c>
       <c r="D702" t="s">
-        <v>1488</v>
+        <v>1487</v>
       </c>
     </row>
     <row r="703">
@@ -14410,7 +14407,7 @@
         <v>1353</v>
       </c>
       <c r="D703" t="s">
-        <v>1498</v>
+        <v>1497</v>
       </c>
     </row>
     <row r="704">
@@ -14438,7 +14435,7 @@
         <v>1355</v>
       </c>
       <c r="D705" t="s">
-        <v>1499</v>
+        <v>1498</v>
       </c>
     </row>
     <row r="706">
@@ -14452,7 +14449,7 @@
         <v>1356</v>
       </c>
       <c r="D706" t="s">
-        <v>1500</v>
+        <v>1499</v>
       </c>
     </row>
     <row r="707">
@@ -14480,7 +14477,7 @@
         <v>1358</v>
       </c>
       <c r="D708" t="s">
-        <v>1501</v>
+        <v>1500</v>
       </c>
     </row>
     <row r="709">
@@ -14494,7 +14491,7 @@
         <v>1359</v>
       </c>
       <c r="D709" t="s">
-        <v>1502</v>
+        <v>1501</v>
       </c>
     </row>
   </sheetData>

</xml_diff>